<commit_message>
Eliminada columna de valores calibrados para Temp y rellenado de tres celdas de temperatura
</commit_message>
<xml_diff>
--- a/EC12_CMGJ.xlsx
+++ b/EC12_CMGJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaime\workspace_v12\mundofisico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C99760-AB7F-4849-8534-FA2A9A75F6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448A76A3-5DA7-4C6B-87CC-E250D415D045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="660" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="57">
   <si>
     <t>Vcc</t>
   </si>
@@ -355,9 +355,6 @@
   </si>
   <si>
     <t>Nideal</t>
-  </si>
-  <si>
-    <t>Nadc_corr</t>
   </si>
   <si>
     <t>Tcalib</t>
@@ -3425,10 +3422,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:N22"/>
+  <dimension ref="B2:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3439,14 +3436,13 @@
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.109375" customWidth="1"/>
     <col min="8" max="8" width="31.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="31.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E3" s="58" t="s">
         <v>27</v>
       </c>
@@ -3457,16 +3453,15 @@
       <c r="J3" s="62"/>
       <c r="K3" s="62"/>
       <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="63"/>
-    </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N6" s="29" t="s">
+      <c r="M3" s="63"/>
+    </row>
+    <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M6" s="29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E7" s="14" t="s">
         <v>24</v>
       </c>
@@ -3483,17 +3478,14 @@
       <c r="J7" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="L7" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" s="24" t="s">
+      <c r="M7" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
@@ -3508,12 +3500,11 @@
       </c>
       <c r="I8" s="49"/>
       <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="N8" s="30" t="s">
+      <c r="M8" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="23" t="s">
         <v>8</v>
       </c>
@@ -3534,20 +3525,19 @@
       </c>
       <c r="I9" s="25"/>
       <c r="J9" s="25">
-        <f>H9*($C$10/2^15)*($C$12/2^15)+$C$9</f>
-        <v>1256.7282925397158</v>
-      </c>
-      <c r="K9" s="25">
         <f>(85-30)*(H9-$C$16)/($C$20-$C$16)+30</f>
         <v>29.753363228699552</v>
       </c>
-      <c r="L9">
-        <f>SUM(K9:K12)/4</f>
+      <c r="K9">
+        <f>SUM(J9:J12)/4</f>
         <v>29.938340807174889</v>
       </c>
-      <c r="N9" s="31"/>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M9" s="31">
+        <f>K9</f>
+        <v>29.938340807174889</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
         <v>11</v>
       </c>
@@ -3568,18 +3558,14 @@
       </c>
       <c r="I10" s="25"/>
       <c r="J10" s="25">
-        <f t="shared" ref="J10:J12" si="0">H10*($C$10/2^15)*($C$12/2^15)+$C$9</f>
-        <v>1256.7282925397158</v>
-      </c>
-      <c r="K10" s="25">
-        <f t="shared" ref="K10:K12" si="1">(85-30)*(H10-$C$16)/($C$20-$C$16)+30</f>
+        <f t="shared" ref="J10:J12" si="0">(85-30)*(H10-$C$16)/($C$20-$C$16)+30</f>
         <v>29.753363228699552</v>
       </c>
-      <c r="N10" s="30" t="s">
+      <c r="M10" s="30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="E11" s="12" t="s">
@@ -3597,15 +3583,14 @@
       <c r="I11" s="25"/>
       <c r="J11" s="25">
         <f t="shared" si="0"/>
-        <v>1260.7147423177958</v>
-      </c>
-      <c r="K11" s="25">
-        <f t="shared" si="1"/>
         <v>30.739910313901344</v>
       </c>
-      <c r="N11" s="31"/>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M11" s="31">
+        <f>K14</f>
+        <v>30.580985915492956</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="22" t="s">
         <v>15</v>
       </c>
@@ -3627,17 +3612,13 @@
       <c r="I12" s="25"/>
       <c r="J12" s="25">
         <f t="shared" si="0"/>
-        <v>1255.7316800951958</v>
-      </c>
-      <c r="K12" s="25">
-        <f t="shared" si="1"/>
         <v>29.506726457399104</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="M12" s="30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="22" t="s">
         <v>14</v>
       </c>
@@ -3652,10 +3633,12 @@
       </c>
       <c r="I13" s="49"/>
       <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M13" s="12">
+        <f>K19</f>
+        <v>30.073333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
         <v>13</v>
       </c>
@@ -3676,19 +3659,15 @@
       </c>
       <c r="I14" s="25"/>
       <c r="J14" s="25">
-        <f>H14*($C$10/2^15)*($C$13/2^15)+$C$9</f>
-        <v>1568.5177145339549</v>
-      </c>
-      <c r="K14" s="25">
         <f>(85-30)*(H14-$C$17)/($C$21-$C$17)+30</f>
         <v>30</v>
       </c>
-      <c r="L14">
-        <f>SUM(K14:K17)/4</f>
+      <c r="K14">
+        <f>SUM(J14:J17)/4</f>
         <v>30.580985915492956</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="3"/>
       <c r="E15" s="12" t="s">
@@ -3705,15 +3684,11 @@
       </c>
       <c r="I15" s="25"/>
       <c r="J15" s="25">
-        <f t="shared" ref="J15:J17" si="2">H15*($C$10/2^15)*($C$13/2^15)+$C$9</f>
-        <v>1577.4072985583916</v>
-      </c>
-      <c r="K15" s="25">
-        <f t="shared" ref="K15:K17" si="3">(85-30)*(H15-$C$17)/($C$21-$C$17)+30</f>
+        <f t="shared" ref="J15:J17" si="1">(85-30)*(H15-$C$17)/($C$21-$C$17)+30</f>
         <v>31.742957746478872</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="20" t="s">
         <v>17</v>
       </c>
@@ -3734,15 +3709,11 @@
       </c>
       <c r="I16" s="25"/>
       <c r="J16" s="25">
-        <f t="shared" si="2"/>
-        <v>1573.4563723253086</v>
-      </c>
-      <c r="K16" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>30.968309859154928</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="20" t="s">
         <v>16</v>
       </c>
@@ -3763,15 +3734,11 @@
       </c>
       <c r="I17" s="25"/>
       <c r="J17" s="25">
-        <f t="shared" si="2"/>
-        <v>1566.5422514174134</v>
-      </c>
-      <c r="K17" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>29.612676056338028</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="20" t="s">
         <v>12</v>
       </c>
@@ -3786,9 +3753,8 @@
       </c>
       <c r="I18" s="49"/>
       <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-    </row>
-    <row r="19" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
       <c r="E19" s="12" t="s">
@@ -3805,19 +3771,15 @@
       </c>
       <c r="I19" s="25"/>
       <c r="J19" s="25">
-        <f>H19*($C$10/2^15)*($C$14/2^15)+$C$9</f>
-        <v>2095.3061292171478</v>
-      </c>
-      <c r="K19" s="25">
         <f>(85-30)*(H19-$C$18)/($C$22-$C$18)+30</f>
         <v>30.733333333333334</v>
       </c>
-      <c r="L19">
-        <f>SUM(K19:K22)/4</f>
+      <c r="K19">
+        <f>SUM(J19:J22)/4</f>
         <v>30.073333333333334</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="21" t="s">
         <v>18</v>
       </c>
@@ -3838,15 +3800,11 @@
       </c>
       <c r="I20" s="25"/>
       <c r="J20" s="25">
-        <f t="shared" ref="J20:J22" si="4">H20*($C$10/2^15)*($C$14/2^15)+$C$9</f>
-        <v>2086.377267871052</v>
-      </c>
-      <c r="K20" s="25">
-        <f t="shared" ref="K20:K22" si="5">(85-30)*(H20-$C$18)/($C$22-$C$18)+30</f>
+        <f t="shared" ref="J20:J22" si="2">(85-30)*(H20-$C$18)/($C$22-$C$18)+30</f>
         <v>29.413333333333334</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
         <v>19</v>
       </c>
@@ -3867,15 +3825,11 @@
       </c>
       <c r="I21" s="25"/>
       <c r="J21" s="25">
-        <f t="shared" si="4"/>
-        <v>2091.3377463966608</v>
-      </c>
-      <c r="K21" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>30.146666666666668</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
         <v>20</v>
       </c>
@@ -3896,17 +3850,13 @@
       </c>
       <c r="I22" s="25"/>
       <c r="J22" s="25">
-        <f t="shared" si="4"/>
-        <v>2090.345650691539</v>
-      </c>
-      <c r="K22" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="E3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>